<commit_message>
back to last success
</commit_message>
<xml_diff>
--- a/output/model_results.xlsx
+++ b/output/model_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1201,54 +1201,6 @@
         <v>0.825045871559633</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>LogisticRegression</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>{'random_state': 42, 'optimize': True, 'n_trials': 5}</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>0.4848541977967454</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.8392316513761467</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.4988093256561148</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.8347706422018348</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>LogisticRegression</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>{'random_state': 42, 'optimize': True, 'n_trials': 5}</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>0.4848541977967454</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.8392316513761467</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.4988093256561148</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.8347706422018348</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
selected model hepsi çalışacak hale getirildi
</commit_message>
<xml_diff>
--- a/output/model_results.xlsx
+++ b/output/model_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1225,6 +1225,78 @@
         <v>0.8287155963302753</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>LogisticRegression</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>{'max_iter': 250}</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.5011377861893516</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.8325917431192661</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.5094879356504962</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.8287155963302753</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>LogisticRegression</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>{'max_iter': 250}</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.5011377861893516</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.8325917431192661</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.5094879356504962</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.8287155963302753</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DecisionTree</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>{'max_depth': 30}</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.05961969743960245</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.9872935779816514</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.443732803030968</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.8844495412844037</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ann logreg lstm completed
</commit_message>
<xml_diff>
--- a/output/model_results.xlsx
+++ b/output/model_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1345,6 +1345,198 @@
         <v>0.8218565583229065</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>LogisticRegression</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>{'learning_rate': 0.001, 'epochs': 10, 'batch_size': 32, 'optimizer_type': 'adam', 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.5397221446037292</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.8218031525611877</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.5395736694335938</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.8220245242118835</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ANN</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>{'hidden_layers': [32], 'dropout_rate': 0.3, 'learning_rate': 0.01, 'epochs': 20, 'batch_size': 64, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0.4079259037971497</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.8522424101829529</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.3547864258289337</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.8685131072998047</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ANN</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>{'hidden_layers': [32], 'dropout_rate': 0.3, 'learning_rate': 0.01, 'epochs': 20, 'batch_size': 64, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.4055112302303314</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.8511757850646973</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.3556340336799622</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.8694465160369873</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>{'time_steps': 8, 'lstm_units': 64, 'epochs': 10, 'batch_size': 90, 'learning_rate': 0.001, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.2662752270698547</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9027020931243896</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.2909113466739655</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.8963072299957275</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ANN</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>{'hidden_layers': [32], 'dropout_rate': 0.3, 'learning_rate': 0.01, 'epochs': 20, 'batch_size': 64, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.4043055474758148</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.8534204959869385</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.3485387563705444</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.8739444017410278</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>{'time_steps': 8, 'lstm_units': 64, 'epochs': 10, 'batch_size': 90, 'learning_rate': 0.001, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.2613523900508881</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.9052728414535522</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.2875173687934875</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.8960378170013428</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>{'time_steps': 8, 'hidden_size': 128, 'num_layers': 3, 'dropout_rate': 0.4, 'epochs': 10, 'batch_size': 90, 'learning_rate': 0.0005, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.3039801716804504</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.8872016668319702</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.3051522970199585</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.8897278904914856</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>{'time_steps': 8, 'lstm_units': 64, 'epochs': 10, 'batch_size': 90, 'learning_rate': 0.001, 'early_stopping': True, 'patience': 10, 'learning_rate_scheduling': True, 'factor': 0.1, 'min_lr': 1e-06}</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.2628472447395325</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.9046638011932373</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.2815037965774536</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.8970574736595154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
time added in feature
</commit_message>
<xml_diff>
--- a/output/model_results.xlsx
+++ b/output/model_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1917,6 +1917,30 @@
         <v>0.857707509881423</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>RandomForest</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_depth': 20, 'random_state': 42}</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0.07107472561565627</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.227799580037436</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.9469226425748165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>